<commit_message>
NAP2 Financial data verif ganti time out
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
+++ b/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
@@ -1649,7 +1649,7 @@
         <v>99</v>
       </c>
       <c r="B2" t="n">
-        <v>1.22605E8</v>
+        <v>3.5062E8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1679,7 +1679,7 @@
         <v>30</v>
       </c>
       <c r="B5" t="n">
-        <v>6.11E8</v>
+        <v>1.002E9</v>
       </c>
       <c r="C5" s="89" t="s">
         <v>94</v>
@@ -1699,7 +1699,7 @@
         <v>100</v>
       </c>
       <c r="B6" t="n">
-        <v>1.2262E8</v>
+        <v>3.5062E8</v>
       </c>
       <c r="C6" s="89" t="s">
         <v>94</v>
@@ -1708,7 +1708,7 @@
         <v>3</v>
       </c>
       <c r="E6" t="n">
-        <v>3.3151E7</v>
+        <v>3.92705E7</v>
       </c>
       <c r="F6" s="89" t="s">
         <v>94</v>
@@ -1717,7 +1717,7 @@
         <v>12</v>
       </c>
       <c r="H6" t="n">
-        <v>2.476125E7</v>
+        <v>2.932525E7</v>
       </c>
       <c r="I6" s="89" t="s">
         <v>94</v>
@@ -1735,7 +1735,7 @@
         <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>4.3455345E7</v>
+        <v>0.0</v>
       </c>
       <c r="F7" s="89" t="s">
         <v>94</v>
@@ -1744,7 +1744,7 @@
         <v>14</v>
       </c>
       <c r="H7" t="n">
-        <v>4.44542E7</v>
+        <v>0.0</v>
       </c>
       <c r="I7" s="89" t="s">
         <v>94</v>
@@ -1755,7 +1755,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="n">
-        <v>0.1468207</v>
+        <v>0.14685478</v>
       </c>
       <c r="C8" s="89" t="s">
         <v>94</v>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="C24" s="25"/>
       <c r="D24" t="n">
-        <v>3.08145E7</v>
+        <v>3.6437E7</v>
       </c>
       <c r="E24" s="89" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
revisi fin data verif MAPcompany hapus take out life ins
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
+++ b/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
@@ -1649,7 +1649,7 @@
         <v>99</v>
       </c>
       <c r="B2" t="n">
-        <v>3.5062E8</v>
+        <v>3.5042E8</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -1657,7 +1657,7 @@
         <v>71</v>
       </c>
       <c r="B3" t="n">
-        <v>7.7217899174E8</v>
+        <v>9.9744298846E8</v>
       </c>
       <c r="C3" s="95" t="s">
         <v>97</v>
@@ -1755,7 +1755,7 @@
         <v>34</v>
       </c>
       <c r="B8" t="n">
-        <v>0.14685478</v>
+        <v>0.14690309</v>
       </c>
       <c r="C8" s="89" t="s">
         <v>94</v>
@@ -1941,7 +1941,7 @@
         <v>42</v>
       </c>
       <c r="B17" t="n">
-        <v>1.354699986E7</v>
+        <v>1.74989998E7</v>
       </c>
       <c r="C17" s="88" t="s">
         <v>93</v>
@@ -2125,7 +2125,7 @@
       </c>
       <c r="C25" s="25"/>
       <c r="D25" t="n">
-        <v>1.3036604E7</v>
+        <v>0.0</v>
       </c>
       <c r="E25" s="89" t="s">
         <v>94</v>

</xml_diff>

<commit_message>
AITATR3-315 + 316 + 318
</commit_message>
<xml_diff>
--- a/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
+++ b/Simulasi/Simulasi Perhitungan Gross Yield & Angsuran Regular Fixed CF.xlsx
@@ -1633,7 +1633,7 @@
   <dimension ref="A1:N85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1795,7 +1795,7 @@
         <v>15</v>
       </c>
       <c r="H8">
-        <v>0</v>
+        <v>29078</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>93</v>
@@ -1824,7 +1824,7 @@
         <v>16</v>
       </c>
       <c r="H9">
-        <v>0</v>
+        <v>1006020</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>93</v>
@@ -2030,7 +2030,7 @@
       </c>
       <c r="J20" s="99">
         <f>IF(B16=0,B37-C37,0)</f>
-        <v>-646479348.84000003</v>
+        <v>-647514446.84000003</v>
       </c>
       <c r="L20" s="13"/>
     </row>
@@ -2429,7 +2429,7 @@
       <c r="B34" s="22"/>
       <c r="C34" s="98">
         <f>H8</f>
-        <v>0</v>
+        <v>29078</v>
       </c>
       <c r="D34" s="20"/>
       <c r="F34" s="104">
@@ -2456,7 +2456,7 @@
       <c r="B35" s="22"/>
       <c r="C35" s="98">
         <f>H9</f>
-        <v>0</v>
+        <v>1006020</v>
       </c>
       <c r="D35" s="20"/>
       <c r="F35" s="104">
@@ -2507,7 +2507,7 @@
       </c>
       <c r="C37" s="16">
         <f>SUM(C21:C35)</f>
-        <v>1009407348.84</v>
+        <v>1010442446.84</v>
       </c>
       <c r="D37" t="s">
         <v>49</v>
@@ -3359,11 +3359,11 @@
       </c>
       <c r="J83" s="55">
         <f ca="1">IRR(J20:INDIRECT(CONCATENATE("J",B13+20)))</f>
-        <v>1.3218412524505618E-2</v>
+        <v>1.3013584578049242E-2</v>
       </c>
       <c r="K83" s="109">
         <f ca="1">J83*(12/B10)*100</f>
-        <v>15.862095029406742</v>
+        <v>15.61630149365909</v>
       </c>
       <c r="L83" s="103"/>
     </row>
@@ -3374,7 +3374,7 @@
       </c>
       <c r="J84">
         <f ca="1">_xlfn.NUMBERVALUE(K83)</f>
-        <v>15.862095029406699</v>
+        <v>15.616301493659099</v>
       </c>
     </row>
     <row r="85" spans="6:13">

</xml_diff>